<commit_message>
correct some dict key bugs
</commit_message>
<xml_diff>
--- a/src/testData/LoansTest.xlsx
+++ b/src/testData/LoansTest.xlsx
@@ -376,7 +376,7 @@
   <dimension ref="A1:AD8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA1" activeCellId="0" sqref="AA1"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -812,7 +812,7 @@
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="4" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -881,7 +881,7 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="4" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>

</xml_diff>

<commit_message>
remove the csv logic, correct the loan counts for geojson
</commit_message>
<xml_diff>
--- a/src/testData/LoansTest.xlsx
+++ b/src/testData/LoansTest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
   <si>
     <t xml:space="preserve">LOAN_NO</t>
   </si>
@@ -173,6 +173,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -298,12 +299,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -373,16 +374,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD8"/>
+  <dimension ref="A1:AD11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1013" min="1" style="0" width="15.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1014" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1014" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -731,7 +731,7 @@
       </c>
       <c r="AD5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>6</v>
       </c>
@@ -745,63 +745,39 @@
       <c r="E6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="F6" s="2"/>
       <c r="G6" s="4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="3" t="n">
         <v>33738</v>
       </c>
-      <c r="K6" s="3" t="n">
-        <v>33739</v>
-      </c>
-      <c r="L6" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="4"/>
       <c r="M6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="N6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O6" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="N6" s="2"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
-      <c r="R6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" s="4" t="n">
-        <v>0</v>
-      </c>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
       <c r="U6" s="2"/>
-      <c r="W6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="4" t="n">
-        <v>0</v>
-      </c>
+      <c r="W6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="4"/>
       <c r="AD6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>7</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>34124</v>
+        <v>33861</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
@@ -812,124 +788,296 @@
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="4" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="3" t="n">
-        <v>34124</v>
-      </c>
-      <c r="K7" s="3" t="n">
-        <v>34151</v>
-      </c>
-      <c r="L7" s="4" t="n">
-        <v>1</v>
-      </c>
+        <v>33861</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="4"/>
       <c r="M7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="N7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
-      <c r="R7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="T7" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
       <c r="U7" s="2"/>
-      <c r="W7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="X7" s="3" t="n">
-        <v>34124</v>
-      </c>
-      <c r="Y7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="4" t="n">
-        <v>0</v>
-      </c>
+      <c r="W7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="4"/>
       <c r="AD7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>8</v>
       </c>
       <c r="B8" s="3" t="n">
-        <v>34085</v>
+        <v>33738</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="G8" s="4" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="3" t="n">
-        <v>34085</v>
+        <v>33738</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <v>33739</v>
       </c>
       <c r="L8" s="4" t="n">
         <v>1</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>37</v>
       </c>
       <c r="O8" s="4" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="4" t="n">
         <v>0</v>
       </c>
       <c r="S8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="T8" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8" s="2"/>
       <c r="W8" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="X8" s="3" t="n">
+      <c r="Y8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>34124</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="3" t="n">
+        <v>34124</v>
+      </c>
+      <c r="K9" s="3" t="n">
+        <v>34151</v>
+      </c>
+      <c r="L9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="T9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="U9" s="2"/>
+      <c r="W9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" s="3" t="n">
+        <v>34124</v>
+      </c>
+      <c r="Y9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>34085</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="3" t="n">
+        <v>34085</v>
+      </c>
+      <c r="L10" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="T10" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="U10" s="2"/>
+      <c r="W10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X10" s="3" t="n">
         <v>34089</v>
       </c>
-      <c r="Y8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="2"/>
+      <c r="Y10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>34085</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="3" t="n">
+        <v>34085</v>
+      </c>
+      <c r="L11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="T11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="U11" s="2"/>
+      <c r="W11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" s="3" t="n">
+        <v>34089</v>
+      </c>
+      <c r="Y11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
simpler algorithm for joining tables, and this one looks correct
</commit_message>
<xml_diff>
--- a/src/testData/LoansTest.xlsx
+++ b/src/testData/LoansTest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
   <si>
     <t xml:space="preserve">LOAN_NO</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t xml:space="preserve">Fossil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I</t>
   </si>
   <si>
     <t xml:space="preserve">Foozball artwork5</t>
@@ -174,7 +177,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -203,13 +206,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -289,7 +285,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -298,19 +294,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -394,10 +386,10 @@
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1016" style="0" width="11.52"/>
   </cols>
@@ -412,7 +404,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -501,625 +493,625 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+      <c r="A2" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="3" t="n">
         <v>43545</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="N2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" s="3" t="s">
+      <c r="H2" s="2"/>
+      <c r="I2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="N2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="5" t="n">
+      <c r="P2" s="2"/>
+      <c r="Q2" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="S2" s="3"/>
-      <c r="T2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="W2" s="3"/>
-      <c r="Y2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="4" t="n">
+      <c r="S2" s="2"/>
+      <c r="T2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" s="2"/>
+      <c r="Y2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="3" t="n">
         <v>43543</v>
       </c>
-      <c r="AD2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="3"/>
+      <c r="AD2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B3" s="3" t="n">
         <v>33784</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="5" t="n">
+      <c r="I3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="4" t="n">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="3" t="n">
         <v>33784</v>
       </c>
-      <c r="N3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="O3" s="3" t="s">
+      <c r="N3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" s="5" t="n">
+      <c r="Q3" s="4" t="n">
         <v>53</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S3" s="3"/>
-      <c r="T3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="W3" s="3"/>
-      <c r="Y3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="3"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" s="2"/>
+      <c r="Y3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+      <c r="A4" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="3" t="n">
         <v>34961</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="5" t="n">
+      <c r="I4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="4" t="n">
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="3" t="n">
         <v>34957</v>
       </c>
-      <c r="M4" s="4" t="n">
+      <c r="M4" s="3" t="n">
         <v>34967</v>
       </c>
-      <c r="N4" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" s="3" t="s">
+      <c r="N4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Q4" s="5" t="n">
+      <c r="Q4" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="R4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S4" s="3"/>
-      <c r="T4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="U4" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="V4" s="5" t="n">
+      <c r="S4" s="2"/>
+      <c r="T4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="V4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="W4" s="3"/>
-      <c r="Y4" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="4" t="n">
+      <c r="W4" s="2"/>
+      <c r="Y4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="3" t="n">
         <v>34964</v>
       </c>
-      <c r="AA4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="3"/>
+      <c r="AA4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="3" t="n">
         <v>33647</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="5" t="n">
+      <c r="H5" s="2"/>
+      <c r="I5" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="4" t="n">
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="3" t="n">
         <v>33647</v>
       </c>
-      <c r="M5" s="4" t="n">
+      <c r="M5" s="3" t="n">
         <v>33829</v>
       </c>
-      <c r="N5" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" s="3" t="s">
+      <c r="N5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Q5" s="5" t="n">
+      <c r="Q5" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="R5" s="3" t="s">
+      <c r="R5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="S5" s="3"/>
-      <c r="T5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="U5" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="W5" s="3"/>
-      <c r="Y5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="3"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="W5" s="2"/>
+      <c r="Y5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+      <c r="A6" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="B6" s="3" t="n">
         <v>33738</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="5" t="n">
+      <c r="H6" s="2"/>
+      <c r="I6" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="4" t="n">
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="3" t="n">
         <v>33738</v>
       </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="3" t="s">
+      <c r="M6" s="3"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="W6" s="3"/>
-      <c r="Y6" s="5"/>
-      <c r="AA6" s="5"/>
-      <c r="AD6" s="5"/>
-      <c r="AE6" s="5"/>
-      <c r="AF6" s="3"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="W6" s="2"/>
+      <c r="Y6" s="4"/>
+      <c r="AA6" s="4"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+      <c r="A7" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="B7" s="4" t="n">
+      <c r="B7" s="3" t="n">
         <v>33861</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="5" t="n">
+      <c r="H7" s="2"/>
+      <c r="I7" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="4" t="n">
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="3" t="n">
         <v>33861</v>
       </c>
-      <c r="M7" s="4"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="3" t="s">
+      <c r="M7" s="3"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="W7" s="3"/>
-      <c r="Y7" s="5"/>
-      <c r="AA7" s="5"/>
-      <c r="AD7" s="5"/>
-      <c r="AE7" s="5"/>
-      <c r="AF7" s="3"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="W7" s="2"/>
+      <c r="Y7" s="4"/>
+      <c r="AA7" s="4"/>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+      <c r="A8" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="3" t="n">
         <v>33738</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="5" t="n">
+      <c r="I8" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="4" t="n">
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="3" t="n">
         <v>33738</v>
       </c>
-      <c r="M8" s="4" t="n">
+      <c r="M8" s="3" t="n">
         <v>33739</v>
       </c>
-      <c r="N8" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="O8" s="3" t="s">
+      <c r="N8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="5" t="n">
+      <c r="Q8" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="R8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="S8" s="3"/>
-      <c r="T8" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="U8" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="W8" s="3"/>
-      <c r="Y8" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="3"/>
+      <c r="R8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="S8" s="2"/>
+      <c r="T8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" s="2"/>
+      <c r="Y8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+      <c r="A9" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="B9" s="4" t="n">
+      <c r="B9" s="3" t="n">
         <v>34124</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="5" t="n">
+      <c r="H9" s="2"/>
+      <c r="I9" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="4" t="n">
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="3" t="n">
         <v>34124</v>
       </c>
-      <c r="M9" s="4" t="n">
+      <c r="M9" s="3" t="n">
         <v>34151</v>
       </c>
-      <c r="N9" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="O9" s="3" t="s">
+      <c r="N9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="P9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Q9" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="S9" s="3"/>
-      <c r="T9" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="U9" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="V9" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="W9" s="3"/>
-      <c r="Y9" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="4" t="n">
+      <c r="Q9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S9" s="2"/>
+      <c r="T9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="V9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="W9" s="2"/>
+      <c r="Y9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="3" t="n">
         <v>34124</v>
       </c>
-      <c r="AA9" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="3"/>
+      <c r="AA9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+      <c r="A10" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="B10" s="4" t="n">
+      <c r="B10" s="3" t="n">
         <v>34085</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="5" t="n">
+      <c r="H10" s="2"/>
+      <c r="I10" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="4" t="n">
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="3" t="n">
         <v>34085</v>
       </c>
-      <c r="N10" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="O10" s="3" t="s">
+      <c r="N10" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="P10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Q10" s="5" t="n">
+      <c r="Q10" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="R10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="S10" s="3"/>
-      <c r="T10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="U10" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="V10" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="W10" s="3"/>
-      <c r="Y10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="4" t="n">
+      <c r="R10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="S10" s="2"/>
+      <c r="T10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="V10" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="W10" s="2"/>
+      <c r="Y10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="3" t="n">
         <v>34089</v>
       </c>
-      <c r="AA10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="3"/>
+      <c r="AA10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+      <c r="A11" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="B11" s="4" t="n">
+      <c r="B11" s="3" t="n">
         <v>34085</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="5" t="n">
+      <c r="H11" s="2"/>
+      <c r="I11" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="4" t="n">
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="3" t="n">
         <v>34085</v>
       </c>
-      <c r="N11" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="O11" s="3" t="s">
+      <c r="N11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="P11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Q11" s="5" t="n">
+      <c r="Q11" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="R11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="S11" s="3"/>
-      <c r="T11" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="U11" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="V11" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="W11" s="3"/>
-      <c r="Y11" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="4" t="n">
+      <c r="R11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="S11" s="2"/>
+      <c r="T11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="V11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="W11" s="2"/>
+      <c r="Y11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="3" t="n">
         <v>34089</v>
       </c>
-      <c r="AA11" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF11" s="3"/>
+      <c r="AA11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>